<commit_message>
pdf html exporter test
</commit_message>
<xml_diff>
--- a/zss.test/src/test/java/org/zkoss/zss/ng/exporter/book/simpleChart.xlsx
+++ b/zss.test/src/test/java/org/zkoss/zss/ng/exporter/book/simpleChart.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>A</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -49,6 +49,10 @@
   </si>
   <si>
     <t>Sunday</t>
+  </si>
+  <si>
+    <t>A2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -367,11 +371,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="45613056"/>
-        <c:axId val="45614592"/>
+        <c:axId val="48627712"/>
+        <c:axId val="48629248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="45613056"/>
+        <c:axId val="48627712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -380,7 +384,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45614592"/>
+        <c:crossAx val="48629248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -388,7 +392,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45614592"/>
+        <c:axId val="48629248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -399,7 +403,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45613056"/>
+        <c:crossAx val="48627712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -743,15 +747,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D16:G24"/>
+  <dimension ref="A2:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="16" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
ignore PDF and HTML exporter test (manual only)
</commit_message>
<xml_diff>
--- a/zss.test/src/test/java/org/zkoss/zss/ng/exporter/book/simpleChart.xlsx
+++ b/zss.test/src/test/java/org/zkoss/zss/ng/exporter/book/simpleChart.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>A</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -49,10 +49,6 @@
   </si>
   <si>
     <t>Sunday</t>
-  </si>
-  <si>
-    <t>A2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -371,11 +367,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="48627712"/>
-        <c:axId val="48629248"/>
+        <c:axId val="171426560"/>
+        <c:axId val="171428096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48627712"/>
+        <c:axId val="171426560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -384,7 +380,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48629248"/>
+        <c:crossAx val="171428096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -392,7 +388,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48629248"/>
+        <c:axId val="171428096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -403,7 +399,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48627712"/>
+        <c:crossAx val="171426560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -431,14 +427,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -747,20 +743,450 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>8</v>
+      </c>
+      <c r="I13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+      <c r="H14">
+        <v>8</v>
+      </c>
+      <c r="I14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
+      <c r="I15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>0</v>
       </c>

</xml_diff>